<commit_message>
pass logic zipper gates and stage buffer finished
</commit_message>
<xml_diff>
--- a/HW6/Results_HW6_DigitalMos.xlsx
+++ b/HW6/Results_HW6_DigitalMos.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dersler\ITU\ELE\ELE-504E\HWs\DigitalMosInteg.Circ.Design\HW6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404A796D-6E6F-4F99-ABB4-52770A6CB6F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F335CC4-3EC4-4360-91C0-86800ED3C4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30825" yWindow="2130" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="results" sheetId="1" r:id="rId1"/>
+    <sheet name="calculations" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>n</t>
   </si>
@@ -36,12 +37,6 @@
     <t>L</t>
   </si>
   <si>
-    <t>3.71</t>
-  </si>
-  <si>
-    <t>0.37ns</t>
-  </si>
-  <si>
     <t>Table 5.1</t>
   </si>
   <si>
@@ -51,18 +46,9 @@
     <t>Tphl</t>
   </si>
   <si>
-    <t>35.43 ns</t>
-  </si>
-  <si>
     <t>Tplh</t>
   </si>
   <si>
-    <t>53.57 ns</t>
-  </si>
-  <si>
-    <t>44.5 ns</t>
-  </si>
-  <si>
     <t>Table 5.2</t>
   </si>
   <si>
@@ -75,40 +61,43 @@
     <t>Wp</t>
   </si>
   <si>
-    <t>0.5um</t>
-  </si>
-  <si>
-    <t>0.75um</t>
-  </si>
-  <si>
-    <t>1.85um</t>
-  </si>
-  <si>
-    <t>6.88um</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.53um </t>
-  </si>
-  <si>
-    <t>94.72um</t>
-  </si>
-  <si>
-    <t>2.78um</t>
-  </si>
-  <si>
-    <t>142.08um</t>
-  </si>
-  <si>
-    <t>351,43um</t>
-  </si>
-  <si>
-    <t>10.32um</t>
-  </si>
-  <si>
-    <t>38.29um</t>
-  </si>
-  <si>
-    <t>527.14um</t>
+    <t>jnmax</t>
+  </si>
+  <si>
+    <t>jpmax</t>
+  </si>
+  <si>
+    <t>cl</t>
+  </si>
+  <si>
+    <t>wn</t>
+  </si>
+  <si>
+    <t>cgso</t>
+  </si>
+  <si>
+    <t>vdd</t>
+  </si>
+  <si>
+    <t>lmin</t>
+  </si>
+  <si>
+    <t>cox</t>
+  </si>
+  <si>
+    <t>wp/wn</t>
+  </si>
+  <si>
+    <t>um</t>
+  </si>
+  <si>
+    <t>Table 5.4</t>
+  </si>
+  <si>
+    <t>Simulated L for Stage Buffer</t>
+  </si>
+  <si>
+    <t>Simulated L for single inverter</t>
   </si>
 </sst>
 </file>
@@ -144,9 +133,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -430,113 +421,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="E1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="L1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
+      <c r="B3">
+        <v>3.07</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="2">
+        <f>F3*1.505</f>
+        <v>0.75249999999999995</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3">
+        <v>1.5049999999999999</v>
+      </c>
+      <c r="L3" s="1">
+        <v>8.6999999999999999E-10</v>
+      </c>
+      <c r="M3" s="1">
+        <v>6.5799999999999994E-8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
+      <c r="B4" s="1">
+        <v>3.73E-10</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F4" s="3">
+        <f>F3*3.07</f>
+        <v>1.5349999999999999</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G9" si="0">F4*1.505</f>
+        <v>2.3101749999999996</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E5">
         <v>3</v>
       </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="F5" s="3">
+        <f t="shared" ref="F5:F9" si="1">F4*3.07</f>
+        <v>4.7124499999999996</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>7.0922372499999993</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
       <c r="E6">
         <v>4</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="3">
+        <f t="shared" si="1"/>
+        <v>14.467221499999997</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>21.773168357499994</v>
+      </c>
+      <c r="H6" t="s">
         <v>20</v>
       </c>
-      <c r="G6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -544,40 +579,200 @@
       <c r="E7">
         <v>5</v>
       </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
+      <c r="F7" s="3">
+        <f t="shared" si="1"/>
+        <v>44.414370004999988</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>66.843626857524981</v>
+      </c>
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <f>(calculations!B4*calculations!B11)/(0.0000005*2*calculations!B9)</f>
+        <v>3.5433070866141732E-8</v>
+      </c>
+      <c r="B8" s="1">
+        <f>(calculations!B4*calculations!B11)/(0.00000075*2*calculations!B10)</f>
+        <v>5.3571428571428564E-8</v>
+      </c>
+      <c r="C8" s="1">
+        <f>(A8+B8)/2</f>
+        <v>4.4502249718785145E-8</v>
       </c>
       <c r="E8">
         <v>6</v>
       </c>
-      <c r="F8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" t="s">
-        <v>27</v>
+      <c r="F8" s="3">
+        <f t="shared" si="1"/>
+        <v>136.35211591534997</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>205.20993445260169</v>
+      </c>
+      <c r="H8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="1"/>
+        <v>418.60099586012439</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>629.99449876948711</v>
+      </c>
+      <c r="H9" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="E1:G1"/>
+    <mergeCell ref="L1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98B22285-FBB4-4EB0-B122-AAC1DBBD81C6}">
+  <dimension ref="A4:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1">
+        <v>9.9999999999999994E-12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4.9999999999999998E-7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1">
+        <v>7.1849999999999995E-10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.9999999999999999E-7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1">
+        <v>8.4290000000000007E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <f>LN(B4/
+(((1+SQRT(B9/B10))*(B7*B8+2*B6)*B5
+)))</f>
+        <v>7.8460933572850315</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1">
+        <f>((B4/
+(((1+SQRT(B9/B10))*(B7*B8+2*B6)*B5
+))))^(1/7)</f>
+        <v>3.0675232579014469</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1">
+        <f>(1/4)*
+(
+(1/SQRT(B9))+(1/SQRT(B10))
+)^2
+*(B7*B8+2*B6)
+*B15*C14*B11</f>
+        <v>3.7300995902695044E-10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <f>SQRT(B9/B10)</f>
+        <v>1.5059406173077154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>